<commit_message>
FIX: Import formatNumber for center label
</commit_message>
<xml_diff>
--- a/data/raw/Iran_Budget_Table_1-2-5-7_1404_Template.xlsx
+++ b/data/raw/Iran_Budget_Table_1-2-5-7_1404_Template.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamidreza/Documents/AI-Projects/IranBudget/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88A7E58-8C31-AC48-B70D-40CD9F38EFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E061A8A-DBCB-0844-8658-387A737366A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8260" yWindow="500" windowWidth="20540" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="500" windowWidth="27460" windowHeight="17500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iran Budget Table 5 - 1404" sheetId="1" r:id="rId1"/>
     <sheet name="Table 1" sheetId="6" r:id="rId2"/>
     <sheet name="table 2" sheetId="2" r:id="rId3"/>
-    <sheet name="table 14" sheetId="3" r:id="rId4"/>
-    <sheet name="Table  7" sheetId="4" r:id="rId5"/>
-    <sheet name="table 8" sheetId="5" r:id="rId6"/>
+    <sheet name="Table 3" sheetId="7" r:id="rId4"/>
+    <sheet name="table 14" sheetId="3" r:id="rId5"/>
+    <sheet name="Table  7" sheetId="4" r:id="rId6"/>
+    <sheet name="table 8" sheetId="5" r:id="rId7"/>
+    <sheet name="Table 11" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet4" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="203">
   <si>
     <t>Classification Code</t>
   </si>
@@ -520,6 +523,132 @@
   </si>
   <si>
     <t>منابع (میلیون ریال)</t>
+  </si>
+  <si>
+    <t>خلاصه واگذاری و تملک دارایی های سرمایه ای در سال ۱۴۰۴</t>
+  </si>
+  <si>
+    <t>واگذاری دارایی های سرمایه ای</t>
+  </si>
+  <si>
+    <t>مبلغ به میلیون ریال</t>
+  </si>
+  <si>
+    <t>بند اول: منبع حاصل از نفت و فرآورده های نفتی</t>
+  </si>
+  <si>
+    <t>بند دوم: منابع حاصل از فروش و واگذاری اموال منقول و غیر منقول</t>
+  </si>
+  <si>
+    <t>بند سوم: منابع حاصل از واگذاری طرح تملک دارایی‌های سرمایه‌ای</t>
+  </si>
+  <si>
+    <t>تملک دارایی‌های سرمایه‌ای</t>
+  </si>
+  <si>
+    <t>خالص دارایی‌های سرمایه‌ای</t>
+  </si>
+  <si>
+    <t>جدول ۱۱ - بودجه مصوب شرکت‌های دولتی سال ۱۴۰۴</t>
+  </si>
+  <si>
+    <t>درآمدها</t>
+  </si>
+  <si>
+    <t>اعتبارات هزینه ای</t>
+  </si>
+  <si>
+    <t>اعتبارات تملک دارایی های سرمایه ای</t>
+  </si>
+  <si>
+    <t>تسهیلات بانکی و سایر وام‌های داخلی</t>
+  </si>
+  <si>
+    <t>وام‌های خارجی</t>
+  </si>
+  <si>
+    <t>دارایی‌های جاری</t>
+  </si>
+  <si>
+    <t>سایر دریافتی</t>
+  </si>
+  <si>
+    <t>هزینه‌ها</t>
+  </si>
+  <si>
+    <t>مالیات</t>
+  </si>
+  <si>
+    <t>سود ویژه ۵۰٪</t>
+  </si>
+  <si>
+    <t>سود سهام</t>
+  </si>
+  <si>
+    <t>سایر حسابهای تخصیص سود</t>
+  </si>
+  <si>
+    <t>بازپرداخت تسهیلات بانکی و سایر وامهای داخلی</t>
+  </si>
+  <si>
+    <t>بازپرداخت وام‌های خارجی</t>
+  </si>
+  <si>
+    <t>وجوه اداره شده</t>
+  </si>
+  <si>
+    <t>بازپرداخت ودیعه، بدهی‌ها و سایر پرداخت‌ها</t>
+  </si>
+  <si>
+    <t>هزینه‌های سرمایه‌ای</t>
+  </si>
+  <si>
+    <t>افزایش دارائی‌های جاری</t>
+  </si>
+  <si>
+    <t xml:space="preserve">جمع </t>
+  </si>
+  <si>
+    <t>کسر میشود: ذخیر استهلاک منظور جاری</t>
+  </si>
+  <si>
+    <t>جدول ۱۲ برنامه هم افزایی و ارتقایی فعالیت ها و تولیدات فرهنگی از محل یک درصد از هرین ههای شرکت های دولتی</t>
+  </si>
+  <si>
+    <t>مجمع عالی حکمت اسلامی</t>
+  </si>
+  <si>
+    <t>بنیاد حفظ آثار و نشر ارزش‌های دفاع مقدس</t>
+  </si>
+  <si>
+    <t>وزارت فرهنگ و ارشاد اسلامی (بنیاد ملی بازی‌های رایانه ای</t>
+  </si>
+  <si>
+    <t>حوزه هنری انقلاب اسلامی</t>
+  </si>
+  <si>
+    <t>کانون پرورش فکری کودکان نوجوانان</t>
+  </si>
+  <si>
+    <t>وزارت فرهنگ و ارشاد اسلامی (سازمان سینمایی)</t>
+  </si>
+  <si>
+    <t>دفتر تبلیغات حوزه‌های علمیه</t>
+  </si>
+  <si>
+    <t>وزارت آموزش و پرورش</t>
+  </si>
+  <si>
+    <t>شورای عالی حوزه های علمیه</t>
+  </si>
+  <si>
+    <t>شورای عالی حوزه‌های علمیه خراسان</t>
+  </si>
+  <si>
+    <t>مساجد کشور</t>
+  </si>
+  <si>
+    <t>ورزش همگانی</t>
   </si>
 </sst>
 </file>
@@ -587,7 +716,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -597,6 +726,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1659,7 +1791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26EE61F7-89E7-F642-8EEB-4A485056F2F6}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -2016,6 +2148,121 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4E5FC6-B932-0340-AA64-87FFF61A19CE}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="44.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9300000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6045000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3249502000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5498000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6006000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6006000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3294502000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF8545D6-F954-7E44-AF13-FC7F43241AF2}">
   <dimension ref="A1:E31"/>
   <sheetViews>
@@ -2343,7 +2590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B6B349-D071-2A46-A684-94E9F442A69F}">
   <dimension ref="A1:I32"/>
   <sheetViews>
@@ -2808,7 +3055,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45949736-DAE5-6D4E-BC19-28D03700900E}">
   <dimension ref="A1:B37"/>
   <sheetViews>
@@ -3107,4 +3354,655 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9057D931-65F8-134E-8864-119AB0985D39}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="E2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>48529309948</v>
+      </c>
+      <c r="C3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="1">
+        <v>50443368890</v>
+      </c>
+      <c r="E3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="1">
+        <v>374345109</v>
+      </c>
+      <c r="C4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="1">
+        <v>227506138</v>
+      </c>
+      <c r="E4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <v>645378602</v>
+      </c>
+      <c r="C5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1564426760</v>
+      </c>
+      <c r="E5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>126794436</v>
+      </c>
+      <c r="C6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2537140328</v>
+      </c>
+      <c r="E6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>4338000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="1">
+        <v>883363003</v>
+      </c>
+      <c r="E7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>1445424025</v>
+      </c>
+      <c r="C8" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" s="1">
+        <v>867260060</v>
+      </c>
+      <c r="E8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>903088517</v>
+      </c>
+      <c r="C9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D9" s="1">
+        <v>7250693821</v>
+      </c>
+      <c r="E9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>23411540</v>
+      </c>
+      <c r="C10" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
+        <v>1002840993</v>
+      </c>
+      <c r="C11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="1">
+        <v>12202723728</v>
+      </c>
+      <c r="C12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="1">
+        <v>522448950</v>
+      </c>
+      <c r="C13" t="s">
+        <v>187</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="1">
+        <v>65780103848</v>
+      </c>
+      <c r="C14" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="1">
+        <v>2006344848</v>
+      </c>
+      <c r="C15" t="s">
+        <v>189</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
+        <v>63773759000</v>
+      </c>
+      <c r="C16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="1">
+        <v>63773759000</v>
+      </c>
+      <c r="E16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAEA614-B3CB-BD45-8834-F19AA2F19DFF}">
+  <dimension ref="A1:H43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="1">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="1">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="1">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="1">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="1">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1400000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="1">
+        <v>82170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="1">
+        <v>700000</v>
+      </c>
+      <c r="G13">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="G14">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>196</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4000000</v>
+      </c>
+      <c r="G15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16" s="1">
+        <v>500000</v>
+      </c>
+      <c r="G16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="1">
+        <v>500000</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="G18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="1">
+        <v>50000</v>
+      </c>
+      <c r="G20">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="1">
+        <f>SUM(B2:B20)</f>
+        <v>15022170</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
+      <c r="G22">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="1">
+        <v>500000</v>
+      </c>
+      <c r="G24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="1">
+        <v>500000</v>
+      </c>
+      <c r="G25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B26" s="1">
+        <v>500000</v>
+      </c>
+      <c r="G26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="1">
+        <v>300000</v>
+      </c>
+      <c r="G27">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2000000</v>
+      </c>
+      <c r="G28">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2000000</v>
+      </c>
+      <c r="G29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>198</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="G30">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>132</v>
+      </c>
+      <c r="B31" s="1">
+        <v>500000</v>
+      </c>
+      <c r="G31">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" s="1">
+        <v>500000</v>
+      </c>
+      <c r="G32">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>199</v>
+      </c>
+      <c r="B33" s="1">
+        <v>900000</v>
+      </c>
+      <c r="G33">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>200</v>
+      </c>
+      <c r="B34" s="1">
+        <v>500000</v>
+      </c>
+      <c r="G34">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="G35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>136</v>
+      </c>
+      <c r="B36" s="1">
+        <v>400000</v>
+      </c>
+      <c r="G36">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" s="4">
+        <v>200000</v>
+      </c>
+      <c r="G37">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="4">
+        <f>SUM(B23:B37)</f>
+        <v>10900000</v>
+      </c>
+      <c r="G38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>201</v>
+      </c>
+      <c r="B40" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="G40">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>202</v>
+      </c>
+      <c r="B41" s="4">
+        <v>4060000</v>
+      </c>
+      <c r="G41">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>400</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>